<commit_message>
added lnu 2020 data
</commit_message>
<xml_diff>
--- a/data/lnu/original_data/APC-Lnu2020.xlsx
+++ b/data/lnu/original_data/APC-Lnu2020.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="93">
   <si>
     <t>institution</t>
   </si>
@@ -331,9 +331,6 @@
   </si>
   <si>
     <t>10.1007/978-3-030-49683-8</t>
-  </si>
-  <si>
-    <t>10.1007/978-3-030-49679-1</t>
   </si>
   <si>
     <t>10.1093/eurheartj/ehaa954</t>
@@ -692,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K77"/>
+  <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:D12"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="112" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -762,7 +759,7 @@
         <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -779,7 +776,7 @@
         <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -796,7 +793,7 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -813,7 +810,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -830,7 +827,7 @@
         <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -847,7 +844,7 @@
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -864,7 +861,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -881,7 +878,7 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -898,7 +895,7 @@
         <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -915,7 +912,7 @@
         <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -926,13 +923,13 @@
         <v>2020</v>
       </c>
       <c r="C12">
-        <v>8692.76</v>
+        <v>9315.4500000000007</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -943,13 +940,13 @@
         <v>2020</v>
       </c>
       <c r="C13">
-        <v>9315.4500000000007</v>
+        <v>9366.1200000000008</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -960,13 +957,13 @@
         <v>2020</v>
       </c>
       <c r="C14">
-        <v>9366.1200000000008</v>
+        <v>9497.49</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -977,13 +974,13 @@
         <v>2020</v>
       </c>
       <c r="C15">
-        <v>9497.49</v>
+        <v>9566.15</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -994,13 +991,13 @@
         <v>2020</v>
       </c>
       <c r="C16">
-        <v>9566.15</v>
+        <v>9844.24</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -1011,13 +1008,13 @@
         <v>2020</v>
       </c>
       <c r="C17">
-        <v>9844.24</v>
+        <v>9962.7999999999993</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -1028,13 +1025,13 @@
         <v>2020</v>
       </c>
       <c r="C18">
-        <v>9962.7999999999993</v>
+        <v>10004.17</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -1045,13 +1042,13 @@
         <v>2020</v>
       </c>
       <c r="C19">
-        <v>10004.17</v>
+        <v>10143.620000000001</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1062,13 +1059,13 @@
         <v>2020</v>
       </c>
       <c r="C20">
-        <v>10143.620000000001</v>
+        <v>10176.66</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1079,13 +1076,13 @@
         <v>2020</v>
       </c>
       <c r="C21">
-        <v>10176.66</v>
+        <v>10313.19</v>
       </c>
       <c r="D21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1096,13 +1093,13 @@
         <v>2020</v>
       </c>
       <c r="C22">
-        <v>10313.19</v>
+        <v>10999.25</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1113,10 +1110,10 @@
         <v>2020</v>
       </c>
       <c r="C23">
-        <v>10999.25</v>
+        <v>11468.76</v>
       </c>
       <c r="D23" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E23" t="s">
         <v>92</v>
@@ -1130,13 +1127,13 @@
         <v>2020</v>
       </c>
       <c r="C24">
-        <v>11468.76</v>
+        <v>11683.54</v>
       </c>
       <c r="D24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E24" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1147,13 +1144,13 @@
         <v>2020</v>
       </c>
       <c r="C25">
-        <v>11683.54</v>
+        <v>11751.12</v>
       </c>
       <c r="D25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1164,13 +1161,13 @@
         <v>2020</v>
       </c>
       <c r="C26">
-        <v>11751.12</v>
+        <v>12073.35</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1181,10 +1178,10 @@
         <v>2020</v>
       </c>
       <c r="C27">
-        <v>12073.35</v>
+        <v>12541.1</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="E27" t="s">
         <v>92</v>
@@ -1198,13 +1195,13 @@
         <v>2020</v>
       </c>
       <c r="C28">
-        <v>12541.1</v>
+        <v>12923.74</v>
       </c>
       <c r="D28" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="E28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1215,10 +1212,10 @@
         <v>2020</v>
       </c>
       <c r="C29">
-        <v>12923.74</v>
+        <v>13214.75</v>
       </c>
       <c r="D29" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="E29" t="s">
         <v>92</v>
@@ -1232,13 +1229,13 @@
         <v>2020</v>
       </c>
       <c r="C30">
-        <v>13214.75</v>
+        <v>13241</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="E30" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1249,13 +1246,13 @@
         <v>2020</v>
       </c>
       <c r="C31">
-        <v>13241</v>
+        <v>13563.26</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="E31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -1266,13 +1263,13 @@
         <v>2020</v>
       </c>
       <c r="C32">
-        <v>13563.26</v>
+        <v>14014.33</v>
       </c>
       <c r="D32" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="E32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
@@ -1283,13 +1280,22 @@
         <v>2020</v>
       </c>
       <c r="C33">
-        <v>14014.33</v>
-      </c>
-      <c r="D33" t="s">
-        <v>34</v>
+        <v>14419.76</v>
       </c>
       <c r="E33" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="F33" t="s">
+        <v>75</v>
+      </c>
+      <c r="G33" t="s">
+        <v>76</v>
+      </c>
+      <c r="H33" t="s">
+        <v>77</v>
+      </c>
+      <c r="K33" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
@@ -1300,22 +1306,13 @@
         <v>2020</v>
       </c>
       <c r="C34">
-        <v>14419.76</v>
+        <v>14562.67</v>
+      </c>
+      <c r="D34" t="s">
+        <v>35</v>
       </c>
       <c r="E34" t="s">
-        <v>92</v>
-      </c>
-      <c r="F34" t="s">
-        <v>75</v>
-      </c>
-      <c r="G34" t="s">
-        <v>76</v>
-      </c>
-      <c r="H34" t="s">
-        <v>77</v>
-      </c>
-      <c r="K34" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
@@ -1326,13 +1323,13 @@
         <v>2020</v>
       </c>
       <c r="C35">
-        <v>14562.67</v>
+        <v>14752.47</v>
       </c>
       <c r="D35" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
@@ -1343,10 +1340,10 @@
         <v>2020</v>
       </c>
       <c r="C36">
-        <v>14752.47</v>
+        <v>15018.54</v>
       </c>
       <c r="D36" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E36" t="s">
         <v>92</v>
@@ -1360,13 +1357,13 @@
         <v>2020</v>
       </c>
       <c r="C37">
-        <v>15018.54</v>
+        <v>15089.02</v>
       </c>
       <c r="D37" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E37" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
@@ -1377,13 +1374,13 @@
         <v>2020</v>
       </c>
       <c r="C38">
-        <v>15089.02</v>
+        <v>15189.98</v>
       </c>
       <c r="D38" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
@@ -1394,13 +1391,13 @@
         <v>2020</v>
       </c>
       <c r="C39">
-        <v>15189.98</v>
+        <v>15360.34</v>
       </c>
       <c r="D39" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
@@ -1411,13 +1408,13 @@
         <v>2020</v>
       </c>
       <c r="C40">
-        <v>15360.34</v>
+        <v>15580.61</v>
       </c>
       <c r="D40" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
@@ -1428,13 +1425,13 @@
         <v>2020</v>
       </c>
       <c r="C41">
-        <v>15580.61</v>
+        <v>15604.03</v>
       </c>
       <c r="D41" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E41" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
@@ -1445,13 +1442,13 @@
         <v>2020</v>
       </c>
       <c r="C42">
-        <v>15604.03</v>
+        <v>15681.24</v>
       </c>
       <c r="D42" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
@@ -1462,13 +1459,13 @@
         <v>2020</v>
       </c>
       <c r="C43">
-        <v>15681.24</v>
+        <v>15824.59</v>
       </c>
       <c r="D43" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E43" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
@@ -1479,10 +1476,10 @@
         <v>2020</v>
       </c>
       <c r="C44">
-        <v>15824.59</v>
+        <v>15911.53</v>
       </c>
       <c r="D44" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E44" t="s">
         <v>92</v>
@@ -1496,13 +1493,22 @@
         <v>2020</v>
       </c>
       <c r="C45">
-        <v>15911.53</v>
-      </c>
-      <c r="D45" t="s">
-        <v>45</v>
+        <v>15954.3</v>
       </c>
       <c r="E45" t="s">
-        <v>93</v>
+        <v>91</v>
+      </c>
+      <c r="F45" t="s">
+        <v>81</v>
+      </c>
+      <c r="G45" t="s">
+        <v>81</v>
+      </c>
+      <c r="H45" t="s">
+        <v>80</v>
+      </c>
+      <c r="K45" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
@@ -1513,22 +1519,13 @@
         <v>2020</v>
       </c>
       <c r="C46">
-        <v>15954.3</v>
+        <v>16310.24</v>
+      </c>
+      <c r="D46" t="s">
+        <v>46</v>
       </c>
       <c r="E46" t="s">
-        <v>92</v>
-      </c>
-      <c r="F46" t="s">
-        <v>81</v>
-      </c>
-      <c r="G46" t="s">
-        <v>81</v>
-      </c>
-      <c r="H46" t="s">
-        <v>80</v>
-      </c>
-      <c r="K46" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
@@ -1539,13 +1536,13 @@
         <v>2020</v>
       </c>
       <c r="C47">
-        <v>16310.24</v>
+        <v>16471.79</v>
       </c>
       <c r="D47" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.35">
@@ -1556,13 +1553,13 @@
         <v>2020</v>
       </c>
       <c r="C48">
-        <v>16471.79</v>
+        <v>16895.12</v>
       </c>
       <c r="D48" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E48" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
@@ -1573,10 +1570,10 @@
         <v>2020</v>
       </c>
       <c r="C49">
-        <v>16895.12</v>
+        <v>17117.009999999998</v>
       </c>
       <c r="D49" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="E49" t="s">
         <v>92</v>
@@ -1590,13 +1587,13 @@
         <v>2020</v>
       </c>
       <c r="C50">
-        <v>17117.009999999998</v>
+        <v>17269.2</v>
       </c>
       <c r="D50" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="E50" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
@@ -1607,13 +1604,13 @@
         <v>2020</v>
       </c>
       <c r="C51">
-        <v>17269.2</v>
+        <v>18035.27</v>
       </c>
       <c r="D51" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E51" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
@@ -1624,10 +1621,10 @@
         <v>2020</v>
       </c>
       <c r="C52">
-        <v>18035.27</v>
+        <v>19262.91</v>
       </c>
       <c r="D52" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E52" t="s">
         <v>92</v>
@@ -1641,13 +1638,13 @@
         <v>2020</v>
       </c>
       <c r="C53">
-        <v>19262.91</v>
+        <v>19284.32</v>
       </c>
       <c r="D53" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E53" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
@@ -1658,13 +1655,13 @@
         <v>2020</v>
       </c>
       <c r="C54">
-        <v>19284.32</v>
+        <v>19629.830000000002</v>
       </c>
       <c r="D54" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E54" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
@@ -1675,13 +1672,13 @@
         <v>2020</v>
       </c>
       <c r="C55">
-        <v>19629.830000000002</v>
+        <v>21272.53</v>
       </c>
       <c r="D55" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E55" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
@@ -1692,10 +1689,10 @@
         <v>2020</v>
       </c>
       <c r="C56">
-        <v>21272.53</v>
+        <v>21291.89</v>
       </c>
       <c r="D56" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E56" t="s">
         <v>92</v>
@@ -1709,13 +1706,13 @@
         <v>2020</v>
       </c>
       <c r="C57">
-        <v>21291.89</v>
+        <v>22165.06</v>
       </c>
       <c r="D57" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E57" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
@@ -1726,13 +1723,13 @@
         <v>2020</v>
       </c>
       <c r="C58">
-        <v>22165.06</v>
+        <v>22502.69</v>
       </c>
       <c r="D58" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="E58" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
@@ -1743,10 +1740,10 @@
         <v>2020</v>
       </c>
       <c r="C59">
-        <v>22502.69</v>
+        <v>22984</v>
       </c>
       <c r="D59" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E59" t="s">
         <v>92</v>
@@ -1760,13 +1757,13 @@
         <v>2020</v>
       </c>
       <c r="C60">
-        <v>22984</v>
+        <v>24973.52</v>
       </c>
       <c r="D60" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E60" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
@@ -1777,13 +1774,13 @@
         <v>2020</v>
       </c>
       <c r="C61">
-        <v>24973.52</v>
+        <v>25278.85</v>
       </c>
       <c r="D61" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="E61" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
@@ -1794,13 +1791,13 @@
         <v>2020</v>
       </c>
       <c r="C62">
-        <v>25278.85</v>
+        <v>25869.439999999999</v>
       </c>
       <c r="D62" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E62" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
@@ -1811,13 +1808,13 @@
         <v>2020</v>
       </c>
       <c r="C63">
-        <v>25869.439999999999</v>
+        <v>26221.67</v>
       </c>
       <c r="D63" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E63" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
@@ -1828,13 +1825,13 @@
         <v>2020</v>
       </c>
       <c r="C64">
-        <v>26221.67</v>
+        <v>26342.62</v>
       </c>
       <c r="D64" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E64" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
@@ -1845,10 +1842,10 @@
         <v>2020</v>
       </c>
       <c r="C65">
-        <v>26342.62</v>
+        <v>27345.5</v>
       </c>
       <c r="D65" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E65" t="s">
         <v>92</v>
@@ -1862,13 +1859,13 @@
         <v>2020</v>
       </c>
       <c r="C66">
-        <v>27345.5</v>
+        <v>28667.65</v>
       </c>
       <c r="D66" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E66" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
@@ -1879,13 +1876,13 @@
         <v>2020</v>
       </c>
       <c r="C67">
-        <v>28667.65</v>
+        <v>28995.85</v>
       </c>
       <c r="D67" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E67" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
@@ -1896,13 +1893,13 @@
         <v>2020</v>
       </c>
       <c r="C68">
-        <v>28995.85</v>
+        <v>30000</v>
       </c>
       <c r="D68" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E68" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
@@ -1913,10 +1910,10 @@
         <v>2020</v>
       </c>
       <c r="C69">
-        <v>30000</v>
+        <v>31229.73</v>
       </c>
       <c r="D69" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E69" t="s">
         <v>92</v>
@@ -1930,13 +1927,13 @@
         <v>2020</v>
       </c>
       <c r="C70">
-        <v>31229.73</v>
+        <v>32819.15</v>
       </c>
       <c r="D70" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="E70" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
@@ -1947,13 +1944,13 @@
         <v>2020</v>
       </c>
       <c r="C71">
-        <v>32819.15</v>
+        <v>34819.199999999997</v>
       </c>
       <c r="D71" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
@@ -1964,13 +1961,13 @@
         <v>2020</v>
       </c>
       <c r="C72">
-        <v>34819.199999999997</v>
+        <v>35330.39</v>
       </c>
       <c r="D72" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="E72" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
@@ -1981,13 +1978,13 @@
         <v>2020</v>
       </c>
       <c r="C73">
-        <v>35330.39</v>
+        <v>44848.44</v>
       </c>
       <c r="D73" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="E73" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
@@ -1998,13 +1995,13 @@
         <v>2020</v>
       </c>
       <c r="C74">
-        <v>44848.44</v>
+        <v>50000</v>
       </c>
       <c r="D74" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E74" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
@@ -2015,47 +2012,13 @@
         <v>2020</v>
       </c>
       <c r="C75">
-        <v>50000</v>
+        <v>38529.32</v>
       </c>
       <c r="D75" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E75" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>67</v>
-      </c>
-      <c r="B76">
-        <v>2020</v>
-      </c>
-      <c r="C76">
-        <v>218239.4</v>
-      </c>
-      <c r="D76" t="s">
-        <v>90</v>
-      </c>
-      <c r="E76" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>67</v>
-      </c>
-      <c r="B77">
-        <v>2020</v>
-      </c>
-      <c r="C77">
-        <v>38529.32</v>
-      </c>
-      <c r="D77" t="s">
-        <v>91</v>
-      </c>
-      <c r="E77" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>